<commit_message>
fixed extra "The" on University of Sussex, 2018
</commit_message>
<xml_diff>
--- a/data/strike.xlsx
+++ b/data/strike.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/richard/Dropbox/Work/strike_data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/richard/Documents/Projects/UCUballots/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6AF96470-B302-0C40-A39E-F11AA9A6D8B4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4DF95DC-B9DA-C342-85A7-C294C67FC5EB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14120" activeTab="5" xr2:uid="{23BE16C5-46D7-3D45-9482-8F5E02156AF4}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14120" xr2:uid="{23BE16C5-46D7-3D45-9482-8F5E02156AF4}"/>
   </bookViews>
   <sheets>
     <sheet name="2018_pension_strike" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1098" uniqueCount="517">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1095" uniqueCount="515">
   <si>
     <t xml:space="preserve">Heriot-Watt University </t>
   </si>
@@ -561,9 +561,6 @@
     <t>University of Edinburgh</t>
   </si>
   <si>
-    <t xml:space="preserve">University of Sussex </t>
-  </si>
-  <si>
     <t xml:space="preserve">The University of Nottingham </t>
   </si>
   <si>
@@ -607,9 +604,6 @@
   </si>
   <si>
     <t>The University of Liverpool</t>
-  </si>
-  <si>
-    <t>The University of Sussex</t>
   </si>
   <si>
     <t>University of Hertfordshire</t>
@@ -2029,9 +2023,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7268CA9B-7F9F-C24D-A570-2158C69F1326}">
   <dimension ref="A1:H70"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A21" sqref="A21"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A51" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A66" sqref="A66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="44.5" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2064,7 +2058,7 @@
         <v>31</v>
       </c>
       <c r="H1" s="10" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="2" spans="1:8" ht="17" x14ac:dyDescent="0.2">
@@ -2449,7 +2443,7 @@
     </row>
     <row r="21" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A21" s="22" t="s">
-        <v>516</v>
+        <v>514</v>
       </c>
       <c r="C21" s="21">
         <v>323</v>
@@ -2466,7 +2460,7 @@
     </row>
     <row r="22" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A22" s="11" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="B22" s="12">
         <v>44</v>
@@ -2606,7 +2600,7 @@
     </row>
     <row r="29" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A29" s="11" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="B29" s="12">
         <v>577</v>
@@ -2626,7 +2620,7 @@
     </row>
     <row r="30" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A30" s="11" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="B30" s="12">
         <v>676</v>
@@ -2646,7 +2640,7 @@
     </row>
     <row r="31" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A31" s="11" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B31" s="12">
         <v>1663</v>
@@ -2686,7 +2680,7 @@
     </row>
     <row r="33" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A33" s="11" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B33" s="12">
         <v>1135</v>
@@ -2766,7 +2760,7 @@
     </row>
     <row r="37" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A37" s="22" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="C37" s="21">
         <v>214</v>
@@ -2863,7 +2857,7 @@
     </row>
     <row r="42" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A42" s="11" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="B42" s="12">
         <v>784</v>
@@ -3023,7 +3017,7 @@
     </row>
     <row r="50" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A50" s="11" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="B50" s="12">
         <v>965</v>
@@ -3043,7 +3037,7 @@
     </row>
     <row r="51" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A51" s="11" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B51" s="12">
         <v>415</v>
@@ -3063,7 +3057,7 @@
     </row>
     <row r="52" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A52" s="11" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B52" s="12">
         <v>485</v>
@@ -3103,7 +3097,7 @@
     </row>
     <row r="54" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A54" s="11" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="B54" s="12">
         <v>706</v>
@@ -3123,7 +3117,7 @@
     </row>
     <row r="55" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A55" s="11" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B55" s="12">
         <v>435</v>
@@ -3143,7 +3137,7 @@
     </row>
     <row r="56" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A56" s="11" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="B56" s="12">
         <v>132</v>
@@ -3163,7 +3157,7 @@
     </row>
     <row r="57" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A57" s="11" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B57" s="12">
         <v>453</v>
@@ -3343,7 +3337,7 @@
     </row>
     <row r="66" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A66" s="11" t="s">
-        <v>174</v>
+        <v>201</v>
       </c>
       <c r="B66" s="12">
         <v>655</v>
@@ -3425,10 +3419,10 @@
       <c r="A70" s="8"/>
       <c r="B70" s="4"/>
       <c r="C70" s="23" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="D70" s="23" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="E70" s="23"/>
       <c r="F70" s="23"/>
@@ -3448,7 +3442,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A43" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A21" sqref="A21"/>
+      <selection pane="bottomLeft" activeCell="A66" sqref="A66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3481,7 +3475,7 @@
         <v>31</v>
       </c>
       <c r="H1" s="24" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="2" spans="1:8" ht="17" x14ac:dyDescent="0.2">
@@ -3866,7 +3860,7 @@
     </row>
     <row r="21" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A21" s="22" t="s">
-        <v>516</v>
+        <v>514</v>
       </c>
       <c r="B21" s="10"/>
       <c r="C21" s="21">
@@ -3884,7 +3878,7 @@
     </row>
     <row r="22" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A22" s="11" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="B22" s="12">
         <v>44</v>
@@ -4184,7 +4178,7 @@
     </row>
     <row r="37" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A37" s="22" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="B37" s="10"/>
       <c r="C37" s="21">
@@ -4442,7 +4436,7 @@
     </row>
     <row r="50" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A50" s="17" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="B50" s="12">
         <v>965</v>
@@ -4462,7 +4456,7 @@
     </row>
     <row r="51" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A51" s="11" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B51" s="12">
         <v>415</v>
@@ -4482,7 +4476,7 @@
     </row>
     <row r="52" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A52" s="11" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B52" s="12">
         <v>485</v>
@@ -4522,7 +4516,7 @@
     </row>
     <row r="54" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A54" s="11" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="B54" s="12">
         <v>706</v>
@@ -4542,7 +4536,7 @@
     </row>
     <row r="55" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A55" s="11" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B55" s="12">
         <v>435</v>
@@ -4562,7 +4556,7 @@
     </row>
     <row r="56" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A56" s="11" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="B56" s="12">
         <v>132</v>
@@ -4582,7 +4576,7 @@
     </row>
     <row r="57" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A57" s="11" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B57" s="12">
         <v>453</v>
@@ -4762,7 +4756,7 @@
     </row>
     <row r="66" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A66" s="17" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="B66" s="12">
         <v>655</v>
@@ -4802,7 +4796,7 @@
     </row>
     <row r="68" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A68" s="17" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="B68" s="12">
         <v>816</v>
@@ -4853,8 +4847,8 @@
   <dimension ref="A1:H69"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <pane ySplit="1" topLeftCell="A24" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A37" sqref="A37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4889,7 +4883,7 @@
         <v>31</v>
       </c>
       <c r="H1" s="4" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="2" spans="1:8" ht="17" x14ac:dyDescent="0.2">
@@ -5154,7 +5148,7 @@
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="B12" s="5">
         <v>78</v>
@@ -5232,7 +5226,7 @@
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="B15" s="3">
         <v>42</v>
@@ -5414,7 +5408,7 @@
     </row>
     <row r="22" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="B22" s="2">
         <v>46</v>
@@ -5648,7 +5642,7 @@
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="B31" s="5">
         <v>1172</v>
@@ -5804,7 +5798,7 @@
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>190</v>
+        <v>201</v>
       </c>
       <c r="B37" s="5">
         <v>832</v>
@@ -6673,8 +6667,8 @@
   <dimension ref="A1:H69"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <pane ySplit="1" topLeftCell="A24" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A37" sqref="A37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -6707,7 +6701,7 @@
         <v>31</v>
       </c>
       <c r="H1" s="4" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="2" spans="1:8" ht="17" x14ac:dyDescent="0.2">
@@ -6972,7 +6966,7 @@
     </row>
     <row r="12" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="B12" s="2">
         <v>78</v>
@@ -7050,7 +7044,7 @@
     </row>
     <row r="15" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="B15" s="2">
         <v>42</v>
@@ -7232,7 +7226,7 @@
     </row>
     <row r="22" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="B22" s="2">
         <v>46</v>
@@ -7466,7 +7460,7 @@
     </row>
     <row r="31" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A31" s="1" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="B31" s="2">
         <v>1172</v>
@@ -7622,7 +7616,7 @@
     </row>
     <row r="37" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A37" s="1" t="s">
-        <v>190</v>
+        <v>201</v>
       </c>
       <c r="B37" s="2">
         <v>832</v>
@@ -8491,8 +8485,8 @@
   <dimension ref="A1:H152"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A30" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A50" sqref="A50"/>
+      <pane ySplit="1" topLeftCell="A75" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A88" sqref="A88"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -8524,7 +8518,7 @@
         <v>31</v>
       </c>
       <c r="H1" s="5" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="2" spans="1:8" ht="17" x14ac:dyDescent="0.2">
@@ -9439,7 +9433,7 @@
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="B37" s="3">
         <v>41</v>
@@ -9881,7 +9875,7 @@
     </row>
     <row r="54" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A54" s="8" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="B54" s="2">
         <v>45</v>
@@ -10115,7 +10109,7 @@
     </row>
     <row r="63" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A63" s="8" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="B63" s="2">
         <v>46</v>
@@ -10219,7 +10213,7 @@
     </row>
     <row r="67" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A67" s="8" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="B67" s="2">
         <v>32</v>
@@ -10583,7 +10577,7 @@
     </row>
     <row r="81" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="B81" s="5">
         <v>1190</v>
@@ -10765,7 +10759,7 @@
     </row>
     <row r="88" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
-        <v>190</v>
+        <v>201</v>
       </c>
       <c r="B88" s="5">
         <v>842</v>
@@ -10791,7 +10785,7 @@
     </row>
     <row r="89" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A89" s="8" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="B89" s="2">
         <v>239</v>
@@ -11441,7 +11435,7 @@
     </row>
     <row r="114" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A114" s="8" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="B114" s="2">
         <v>513</v>
@@ -12117,7 +12111,7 @@
     </row>
     <row r="140" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A140" s="8" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="B140" s="2">
         <v>704</v>
@@ -12351,7 +12345,7 @@
     </row>
     <row r="149" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A149" s="8" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="B149" s="2">
         <v>207</v>
@@ -12403,7 +12397,7 @@
     </row>
     <row r="151" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A151" s="8" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="B151" s="2">
         <v>73</v>
@@ -12465,9 +12459,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{106B3507-83EA-2640-8EA8-BF46076DF76B}">
   <dimension ref="A1:K152"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A107" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A114" sqref="A114"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A75" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A88" sqref="A88"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -12499,7 +12493,7 @@
         <v>31</v>
       </c>
       <c r="H1" s="25" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="2" spans="1:8" ht="17" x14ac:dyDescent="0.2">
@@ -13417,7 +13411,7 @@
     </row>
     <row r="37" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A37" s="1" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="B37" s="2">
         <v>41</v>
@@ -13859,7 +13853,7 @@
     </row>
     <row r="54" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A54" s="1" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="B54" s="2">
         <v>45</v>
@@ -14093,7 +14087,7 @@
     </row>
     <row r="63" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A63" s="1" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="B63" s="2">
         <v>46</v>
@@ -14197,7 +14191,7 @@
     </row>
     <row r="67" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A67" s="1" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="B67" s="2">
         <v>32</v>
@@ -14561,7 +14555,7 @@
     </row>
     <row r="81" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A81" s="1" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="B81" s="2">
         <v>1190</v>
@@ -14743,7 +14737,7 @@
     </row>
     <row r="88" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A88" s="1" t="s">
-        <v>190</v>
+        <v>201</v>
       </c>
       <c r="B88" s="2">
         <v>842</v>
@@ -14769,7 +14763,7 @@
     </row>
     <row r="89" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A89" s="1" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="B89" s="2">
         <v>239</v>
@@ -15419,7 +15413,7 @@
     </row>
     <row r="114" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A114" s="1" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="B114" s="2">
         <v>513</v>
@@ -16095,7 +16089,7 @@
     </row>
     <row r="140" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A140" s="1" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="B140" s="2">
         <v>704</v>
@@ -16329,7 +16323,7 @@
     </row>
     <row r="149" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A149" s="1" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="B149" s="2">
         <v>207</v>
@@ -16381,7 +16375,7 @@
     </row>
     <row r="151" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A151" s="8" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="B151" s="2">
         <v>73</v>
@@ -16441,11 +16435,11 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0658826B-A2AD-8D4F-8E05-A10691276418}">
-  <dimension ref="A1:C158"/>
+  <dimension ref="A1:C157"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A40" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A52" sqref="A52"/>
+      <pane ySplit="1" topLeftCell="A78" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A91" sqref="A91:XFD91"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -16459,10 +16453,10 @@
         <v>13</v>
       </c>
       <c r="B1" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="C1" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="17" x14ac:dyDescent="0.2">
@@ -16470,10 +16464,10 @@
         <v>32</v>
       </c>
       <c r="B2" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="C2" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="17" x14ac:dyDescent="0.2">
@@ -16481,10 +16475,10 @@
         <v>94</v>
       </c>
       <c r="B3" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="C3" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="17" x14ac:dyDescent="0.2">
@@ -16492,10 +16486,10 @@
         <v>95</v>
       </c>
       <c r="B4" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="C4" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="17" x14ac:dyDescent="0.2">
@@ -16503,10 +16497,10 @@
         <v>33</v>
       </c>
       <c r="B5" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="C5" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="17" x14ac:dyDescent="0.2">
@@ -16514,10 +16508,10 @@
         <v>34</v>
       </c>
       <c r="B6" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="C6" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="17" x14ac:dyDescent="0.2">
@@ -16525,10 +16519,10 @@
         <v>96</v>
       </c>
       <c r="B7" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="C7" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="17" x14ac:dyDescent="0.2">
@@ -16536,10 +16530,10 @@
         <v>97</v>
       </c>
       <c r="B8" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="C8" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="17" x14ac:dyDescent="0.2">
@@ -16547,10 +16541,10 @@
         <v>98</v>
       </c>
       <c r="B9" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="C9" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="17" x14ac:dyDescent="0.2">
@@ -16558,10 +16552,10 @@
         <v>35</v>
       </c>
       <c r="B10" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="C10" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
     </row>
     <row r="11" spans="1:3" ht="17" x14ac:dyDescent="0.2">
@@ -16569,10 +16563,10 @@
         <v>99</v>
       </c>
       <c r="B11" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="C11" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
     </row>
     <row r="12" spans="1:3" ht="17" x14ac:dyDescent="0.2">
@@ -16580,10 +16574,10 @@
         <v>100</v>
       </c>
       <c r="B12" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="C12" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
     </row>
     <row r="13" spans="1:3" ht="17" x14ac:dyDescent="0.2">
@@ -16591,10 +16585,10 @@
         <v>101</v>
       </c>
       <c r="B13" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="C13" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
     </row>
     <row r="14" spans="1:3" ht="17" x14ac:dyDescent="0.2">
@@ -16602,10 +16596,10 @@
         <v>36</v>
       </c>
       <c r="B14" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="C14" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
     </row>
     <row r="15" spans="1:3" ht="17" x14ac:dyDescent="0.2">
@@ -16613,10 +16607,10 @@
         <v>37</v>
       </c>
       <c r="B15" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="C15" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
     </row>
     <row r="16" spans="1:3" ht="17" x14ac:dyDescent="0.2">
@@ -16624,10 +16618,10 @@
         <v>102</v>
       </c>
       <c r="B16" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="C16" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
     </row>
     <row r="17" spans="1:3" ht="17" x14ac:dyDescent="0.2">
@@ -16635,10 +16629,10 @@
         <v>38</v>
       </c>
       <c r="B17" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="C17" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
     </row>
     <row r="18" spans="1:3" ht="17" x14ac:dyDescent="0.2">
@@ -16646,10 +16640,10 @@
         <v>103</v>
       </c>
       <c r="B18" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="C18" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
     </row>
     <row r="19" spans="1:3" ht="17" x14ac:dyDescent="0.2">
@@ -16657,10 +16651,10 @@
         <v>39</v>
       </c>
       <c r="B19" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="C19" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
     </row>
     <row r="20" spans="1:3" ht="17" x14ac:dyDescent="0.2">
@@ -16668,10 +16662,10 @@
         <v>104</v>
       </c>
       <c r="B20" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="C20" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
     </row>
     <row r="21" spans="1:3" ht="17" x14ac:dyDescent="0.2">
@@ -16679,10 +16673,10 @@
         <v>105</v>
       </c>
       <c r="B21" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="C21" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
     </row>
     <row r="22" spans="1:3" ht="17" x14ac:dyDescent="0.2">
@@ -16690,10 +16684,10 @@
         <v>106</v>
       </c>
       <c r="B22" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="C22" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
     </row>
     <row r="23" spans="1:3" ht="17" x14ac:dyDescent="0.2">
@@ -16701,10 +16695,10 @@
         <v>107</v>
       </c>
       <c r="B23" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="C23" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
     </row>
     <row r="24" spans="1:3" ht="17" x14ac:dyDescent="0.2">
@@ -16712,10 +16706,10 @@
         <v>108</v>
       </c>
       <c r="B24" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="C24" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
     </row>
     <row r="25" spans="1:3" ht="17" x14ac:dyDescent="0.2">
@@ -16723,10 +16717,10 @@
         <v>109</v>
       </c>
       <c r="B25" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="C25" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
     </row>
     <row r="26" spans="1:3" ht="17" x14ac:dyDescent="0.2">
@@ -16734,10 +16728,10 @@
         <v>40</v>
       </c>
       <c r="B26" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="C26" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
     </row>
     <row r="27" spans="1:3" ht="17" x14ac:dyDescent="0.2">
@@ -16745,32 +16739,32 @@
         <v>41</v>
       </c>
       <c r="B27" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="C27" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
     </row>
     <row r="28" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A28" s="27" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="B28" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="C28" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
     </row>
     <row r="29" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A29" s="27" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="B29" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="C29" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
     </row>
     <row r="30" spans="1:3" ht="17" x14ac:dyDescent="0.2">
@@ -16778,10 +16772,10 @@
         <v>42</v>
       </c>
       <c r="B30" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="C30" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
     </row>
     <row r="31" spans="1:3" ht="17" x14ac:dyDescent="0.2">
@@ -16789,10 +16783,10 @@
         <v>43</v>
       </c>
       <c r="B31" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="C31" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
     </row>
     <row r="32" spans="1:3" ht="17" x14ac:dyDescent="0.2">
@@ -16800,10 +16794,10 @@
         <v>110</v>
       </c>
       <c r="B32" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="C32" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
     </row>
     <row r="33" spans="1:3" ht="17" x14ac:dyDescent="0.2">
@@ -16811,10 +16805,10 @@
         <v>111</v>
       </c>
       <c r="B33" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="C33" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
     </row>
     <row r="34" spans="1:3" ht="17" x14ac:dyDescent="0.2">
@@ -16822,10 +16816,10 @@
         <v>112</v>
       </c>
       <c r="B34" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="C34" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
     </row>
     <row r="35" spans="1:3" ht="17" x14ac:dyDescent="0.2">
@@ -16833,10 +16827,10 @@
         <v>113</v>
       </c>
       <c r="B35" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="C35" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
     </row>
     <row r="36" spans="1:3" ht="17" x14ac:dyDescent="0.2">
@@ -16844,10 +16838,10 @@
         <v>114</v>
       </c>
       <c r="B36" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="C36" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
     </row>
     <row r="37" spans="1:3" ht="17" x14ac:dyDescent="0.2">
@@ -16855,10 +16849,10 @@
         <v>115</v>
       </c>
       <c r="B37" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="C37" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
     </row>
     <row r="38" spans="1:3" ht="17" x14ac:dyDescent="0.2">
@@ -16866,21 +16860,21 @@
         <v>116</v>
       </c>
       <c r="B38" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="C38" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
     </row>
     <row r="39" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A39" s="27" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="B39" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="C39" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
     </row>
     <row r="40" spans="1:3" ht="17" x14ac:dyDescent="0.2">
@@ -16888,10 +16882,10 @@
         <v>117</v>
       </c>
       <c r="B40" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="C40" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
     </row>
     <row r="41" spans="1:3" ht="17" x14ac:dyDescent="0.2">
@@ -16899,10 +16893,10 @@
         <v>44</v>
       </c>
       <c r="B41" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="C41" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
     </row>
     <row r="42" spans="1:3" ht="17" x14ac:dyDescent="0.2">
@@ -16910,10 +16904,10 @@
         <v>45</v>
       </c>
       <c r="B42" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="C42" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
     </row>
     <row r="43" spans="1:3" ht="17" x14ac:dyDescent="0.2">
@@ -16921,10 +16915,10 @@
         <v>118</v>
       </c>
       <c r="B43" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="C43" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
     </row>
     <row r="44" spans="1:3" ht="17" x14ac:dyDescent="0.2">
@@ -16932,10 +16926,10 @@
         <v>46</v>
       </c>
       <c r="B44" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="C44" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
     </row>
     <row r="45" spans="1:3" ht="17" x14ac:dyDescent="0.2">
@@ -16943,10 +16937,10 @@
         <v>119</v>
       </c>
       <c r="B45" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="C45" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
     </row>
     <row r="46" spans="1:3" ht="17" x14ac:dyDescent="0.2">
@@ -16954,10 +16948,10 @@
         <v>120</v>
       </c>
       <c r="B46" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="C46" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
     </row>
     <row r="47" spans="1:3" ht="17" x14ac:dyDescent="0.2">
@@ -16965,10 +16959,10 @@
         <v>47</v>
       </c>
       <c r="B47" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="C47" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
     </row>
     <row r="48" spans="1:3" ht="17" x14ac:dyDescent="0.2">
@@ -16976,10 +16970,10 @@
         <v>121</v>
       </c>
       <c r="B48" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="C48" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
     </row>
     <row r="49" spans="1:3" ht="17" x14ac:dyDescent="0.2">
@@ -16987,10 +16981,10 @@
         <v>122</v>
       </c>
       <c r="B49" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="C49" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
     </row>
     <row r="50" spans="1:3" ht="17" x14ac:dyDescent="0.2">
@@ -16998,10 +16992,10 @@
         <v>123</v>
       </c>
       <c r="B50" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="C50" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
     </row>
     <row r="51" spans="1:3" ht="17" x14ac:dyDescent="0.2">
@@ -17009,10 +17003,10 @@
         <v>124</v>
       </c>
       <c r="B51" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="C51" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
     </row>
     <row r="52" spans="1:3" ht="17" x14ac:dyDescent="0.2">
@@ -17020,10 +17014,10 @@
         <v>48</v>
       </c>
       <c r="B52" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="C52" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
     </row>
     <row r="53" spans="1:3" ht="17" x14ac:dyDescent="0.2">
@@ -17031,10 +17025,10 @@
         <v>125</v>
       </c>
       <c r="B53" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="C53" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
     </row>
     <row r="54" spans="1:3" ht="17" x14ac:dyDescent="0.2">
@@ -17042,10 +17036,10 @@
         <v>126</v>
       </c>
       <c r="B54" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="C54" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
     </row>
     <row r="55" spans="1:3" ht="17" x14ac:dyDescent="0.2">
@@ -17053,21 +17047,21 @@
         <v>49</v>
       </c>
       <c r="B55" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="C55" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
     </row>
     <row r="56" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A56" s="27" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="B56" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="C56" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
     </row>
     <row r="57" spans="1:3" ht="17" x14ac:dyDescent="0.2">
@@ -17075,10 +17069,10 @@
         <v>127</v>
       </c>
       <c r="B57" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="C57" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
     </row>
     <row r="58" spans="1:3" ht="17" x14ac:dyDescent="0.2">
@@ -17086,10 +17080,10 @@
         <v>128</v>
       </c>
       <c r="B58" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="C58" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
     </row>
     <row r="59" spans="1:3" ht="17" x14ac:dyDescent="0.2">
@@ -17097,10 +17091,10 @@
         <v>129</v>
       </c>
       <c r="B59" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="C59" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
     </row>
     <row r="60" spans="1:3" ht="17" x14ac:dyDescent="0.2">
@@ -17108,10 +17102,10 @@
         <v>130</v>
       </c>
       <c r="B60" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="C60" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
     </row>
     <row r="61" spans="1:3" ht="17" x14ac:dyDescent="0.2">
@@ -17119,10 +17113,10 @@
         <v>131</v>
       </c>
       <c r="B61" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="C61" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
     </row>
     <row r="62" spans="1:3" ht="17" x14ac:dyDescent="0.2">
@@ -17130,10 +17124,10 @@
         <v>132</v>
       </c>
       <c r="B62" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="C62" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
     </row>
     <row r="63" spans="1:3" ht="17" x14ac:dyDescent="0.2">
@@ -17141,10 +17135,10 @@
         <v>133</v>
       </c>
       <c r="B63" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
       <c r="C63" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
     </row>
     <row r="64" spans="1:3" ht="17" x14ac:dyDescent="0.2">
@@ -17152,21 +17146,21 @@
         <v>134</v>
       </c>
       <c r="B64" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
       <c r="C64" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
     </row>
     <row r="65" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A65" s="27" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="B65" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
       <c r="C65" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
     </row>
     <row r="66" spans="1:3" ht="17" x14ac:dyDescent="0.2">
@@ -17174,21 +17168,21 @@
         <v>50</v>
       </c>
       <c r="B66" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="C66" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
     </row>
     <row r="67" spans="1:3" ht="34" x14ac:dyDescent="0.2">
       <c r="A67" s="27" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="B67" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="C67" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
     </row>
     <row r="68" spans="1:3" ht="17" x14ac:dyDescent="0.2">
@@ -17196,10 +17190,10 @@
         <v>135</v>
       </c>
       <c r="B68" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
       <c r="C68" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
     </row>
     <row r="69" spans="1:3" ht="17" x14ac:dyDescent="0.2">
@@ -17207,21 +17201,21 @@
         <v>136</v>
       </c>
       <c r="B69" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
       <c r="C69" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
     </row>
     <row r="70" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A70" s="27" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="B70" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="C70" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
     </row>
     <row r="71" spans="1:3" ht="17" x14ac:dyDescent="0.2">
@@ -17229,10 +17223,10 @@
         <v>137</v>
       </c>
       <c r="B71" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="C71" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
     </row>
     <row r="72" spans="1:3" ht="17" x14ac:dyDescent="0.2">
@@ -17240,10 +17234,10 @@
         <v>138</v>
       </c>
       <c r="B72" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
       <c r="C72" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
     </row>
     <row r="73" spans="1:3" ht="17" x14ac:dyDescent="0.2">
@@ -17251,10 +17245,10 @@
         <v>139</v>
       </c>
       <c r="B73" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="C73" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
     </row>
     <row r="74" spans="1:3" ht="17" x14ac:dyDescent="0.2">
@@ -17262,10 +17256,10 @@
         <v>51</v>
       </c>
       <c r="B74" t="s">
-        <v>352</v>
+        <v>350</v>
       </c>
       <c r="C74" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
     </row>
     <row r="75" spans="1:3" ht="17" x14ac:dyDescent="0.2">
@@ -17273,10 +17267,10 @@
         <v>52</v>
       </c>
       <c r="B75" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
       <c r="C75" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
     </row>
     <row r="76" spans="1:3" ht="17" x14ac:dyDescent="0.2">
@@ -17284,10 +17278,10 @@
         <v>140</v>
       </c>
       <c r="B76" t="s">
-        <v>356</v>
+        <v>354</v>
       </c>
       <c r="C76" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
     </row>
     <row r="77" spans="1:3" ht="17" x14ac:dyDescent="0.2">
@@ -17295,10 +17289,10 @@
         <v>53</v>
       </c>
       <c r="B77" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
       <c r="C77" t="s">
-        <v>359</v>
+        <v>357</v>
       </c>
     </row>
     <row r="78" spans="1:3" ht="17" x14ac:dyDescent="0.2">
@@ -17306,10 +17300,10 @@
         <v>141</v>
       </c>
       <c r="B78" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
       <c r="C78" t="s">
-        <v>361</v>
+        <v>359</v>
       </c>
     </row>
     <row r="79" spans="1:3" ht="17" x14ac:dyDescent="0.2">
@@ -17317,10 +17311,10 @@
         <v>54</v>
       </c>
       <c r="B79" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
       <c r="C79" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
     </row>
     <row r="80" spans="1:3" ht="17" x14ac:dyDescent="0.2">
@@ -17328,10 +17322,10 @@
         <v>142</v>
       </c>
       <c r="B80" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
       <c r="C80" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
     </row>
     <row r="81" spans="1:3" ht="17" x14ac:dyDescent="0.2">
@@ -17339,10 +17333,10 @@
         <v>55</v>
       </c>
       <c r="B81" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
       <c r="C81" t="s">
-        <v>367</v>
+        <v>365</v>
       </c>
     </row>
     <row r="82" spans="1:3" ht="17" x14ac:dyDescent="0.2">
@@ -17350,10 +17344,10 @@
         <v>56</v>
       </c>
       <c r="B82" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
       <c r="C82" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
     </row>
     <row r="83" spans="1:3" ht="17" x14ac:dyDescent="0.2">
@@ -17361,21 +17355,21 @@
         <v>57</v>
       </c>
       <c r="B83" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
       <c r="C83" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
     </row>
     <row r="84" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A84" s="27" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="B84" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="C84" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
     </row>
     <row r="85" spans="1:3" ht="17" x14ac:dyDescent="0.2">
@@ -17383,10 +17377,10 @@
         <v>58</v>
       </c>
       <c r="B85" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
       <c r="C85" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
     </row>
     <row r="86" spans="1:3" ht="17" x14ac:dyDescent="0.2">
@@ -17394,10 +17388,10 @@
         <v>143</v>
       </c>
       <c r="B86" t="s">
-        <v>376</v>
+        <v>374</v>
       </c>
       <c r="C86" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
     </row>
     <row r="87" spans="1:3" ht="17" x14ac:dyDescent="0.2">
@@ -17405,10 +17399,10 @@
         <v>59</v>
       </c>
       <c r="B87" t="s">
-        <v>378</v>
+        <v>376</v>
       </c>
       <c r="C87" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
     </row>
     <row r="88" spans="1:3" ht="17" x14ac:dyDescent="0.2">
@@ -17416,10 +17410,10 @@
         <v>60</v>
       </c>
       <c r="B88" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
       <c r="C88" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
     </row>
     <row r="89" spans="1:3" ht="17" x14ac:dyDescent="0.2">
@@ -17427,10 +17421,10 @@
         <v>61</v>
       </c>
       <c r="B89" t="s">
-        <v>382</v>
+        <v>380</v>
       </c>
       <c r="C89" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
     </row>
     <row r="90" spans="1:3" ht="17" x14ac:dyDescent="0.2">
@@ -17438,15 +17432,15 @@
         <v>62</v>
       </c>
       <c r="B90" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
       <c r="C90" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
     </row>
     <row r="91" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A91" s="27" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="B91" t="s">
         <v>386</v>
@@ -17457,7 +17451,7 @@
     </row>
     <row r="92" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A92" s="27" t="s">
-        <v>193</v>
+        <v>144</v>
       </c>
       <c r="B92" t="s">
         <v>388</v>
@@ -17468,7 +17462,7 @@
     </row>
     <row r="93" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A93" s="27" t="s">
-        <v>144</v>
+        <v>63</v>
       </c>
       <c r="B93" t="s">
         <v>390</v>
@@ -17479,7 +17473,7 @@
     </row>
     <row r="94" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A94" s="27" t="s">
-        <v>63</v>
+        <v>145</v>
       </c>
       <c r="B94" t="s">
         <v>392</v>
@@ -17490,7 +17484,7 @@
     </row>
     <row r="95" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A95" s="27" t="s">
-        <v>145</v>
+        <v>64</v>
       </c>
       <c r="B95" t="s">
         <v>394</v>
@@ -17501,7 +17495,7 @@
     </row>
     <row r="96" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A96" s="27" t="s">
-        <v>64</v>
+        <v>146</v>
       </c>
       <c r="B96" t="s">
         <v>396</v>
@@ -17512,7 +17506,7 @@
     </row>
     <row r="97" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A97" s="27" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="B97" t="s">
         <v>398</v>
@@ -17523,7 +17517,7 @@
     </row>
     <row r="98" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A98" s="27" t="s">
-        <v>147</v>
+        <v>65</v>
       </c>
       <c r="B98" t="s">
         <v>400</v>
@@ -17534,7 +17528,7 @@
     </row>
     <row r="99" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A99" s="27" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="B99" t="s">
         <v>402</v>
@@ -17545,7 +17539,7 @@
     </row>
     <row r="100" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A100" s="27" t="s">
-        <v>66</v>
+        <v>148</v>
       </c>
       <c r="B100" t="s">
         <v>404</v>
@@ -17556,7 +17550,7 @@
     </row>
     <row r="101" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A101" s="27" t="s">
-        <v>148</v>
+        <v>67</v>
       </c>
       <c r="B101" t="s">
         <v>406</v>
@@ -17567,7 +17561,7 @@
     </row>
     <row r="102" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A102" s="27" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="B102" t="s">
         <v>408</v>
@@ -17578,7 +17572,7 @@
     </row>
     <row r="103" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A103" s="27" t="s">
-        <v>68</v>
+        <v>149</v>
       </c>
       <c r="B103" t="s">
         <v>410</v>
@@ -17589,7 +17583,7 @@
     </row>
     <row r="104" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A104" s="27" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="B104" t="s">
         <v>412</v>
@@ -17600,7 +17594,7 @@
     </row>
     <row r="105" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A105" s="27" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="B105" t="s">
         <v>414</v>
@@ -17611,7 +17605,7 @@
     </row>
     <row r="106" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A106" s="27" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="B106" t="s">
         <v>416</v>
@@ -17622,21 +17616,21 @@
     </row>
     <row r="107" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A107" s="27" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="B107" t="s">
+        <v>376</v>
+      </c>
+      <c r="C107" t="s">
         <v>418</v>
-      </c>
-      <c r="C107" t="s">
-        <v>419</v>
       </c>
     </row>
     <row r="108" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A108" s="27" t="s">
-        <v>153</v>
+        <v>69</v>
       </c>
       <c r="B108" t="s">
-        <v>378</v>
+        <v>419</v>
       </c>
       <c r="C108" t="s">
         <v>420</v>
@@ -17644,7 +17638,7 @@
     </row>
     <row r="109" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A109" s="27" t="s">
-        <v>69</v>
+        <v>154</v>
       </c>
       <c r="B109" t="s">
         <v>421</v>
@@ -17655,7 +17649,7 @@
     </row>
     <row r="110" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A110" s="27" t="s">
-        <v>154</v>
+        <v>173</v>
       </c>
       <c r="B110" t="s">
         <v>423</v>
@@ -17666,7 +17660,7 @@
     </row>
     <row r="111" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A111" s="27" t="s">
-        <v>173</v>
+        <v>71</v>
       </c>
       <c r="B111" t="s">
         <v>425</v>
@@ -17677,7 +17671,7 @@
     </row>
     <row r="112" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A112" s="27" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="B112" t="s">
         <v>427</v>
@@ -17688,7 +17682,7 @@
     </row>
     <row r="113" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A113" s="27" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="B113" t="s">
         <v>429</v>
@@ -17699,7 +17693,7 @@
     </row>
     <row r="114" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A114" s="27" t="s">
-        <v>73</v>
+        <v>155</v>
       </c>
       <c r="B114" t="s">
         <v>431</v>
@@ -17710,7 +17704,7 @@
     </row>
     <row r="115" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A115" s="27" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="B115" t="s">
         <v>433</v>
@@ -17721,7 +17715,7 @@
     </row>
     <row r="116" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A116" s="27" t="s">
-        <v>156</v>
+        <v>189</v>
       </c>
       <c r="B116" t="s">
         <v>435</v>
@@ -17732,7 +17726,7 @@
     </row>
     <row r="117" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A117" s="27" t="s">
-        <v>191</v>
+        <v>74</v>
       </c>
       <c r="B117" t="s">
         <v>437</v>
@@ -17743,7 +17737,7 @@
     </row>
     <row r="118" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A118" s="27" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="B118" t="s">
         <v>439</v>
@@ -17754,7 +17748,7 @@
     </row>
     <row r="119" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A119" s="27" t="s">
-        <v>75</v>
+        <v>157</v>
       </c>
       <c r="B119" t="s">
         <v>441</v>
@@ -17765,29 +17759,29 @@
     </row>
     <row r="120" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A120" s="27" t="s">
-        <v>157</v>
+        <v>179</v>
       </c>
       <c r="B120" t="s">
-        <v>443</v>
+        <v>370</v>
       </c>
       <c r="C120" t="s">
-        <v>444</v>
+        <v>371</v>
       </c>
     </row>
     <row r="121" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A121" s="27" t="s">
-        <v>180</v>
+        <v>76</v>
       </c>
       <c r="B121" t="s">
-        <v>372</v>
+        <v>443</v>
       </c>
       <c r="C121" t="s">
-        <v>373</v>
+        <v>444</v>
       </c>
     </row>
     <row r="122" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A122" s="27" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="B122" t="s">
         <v>445</v>
@@ -17798,7 +17792,7 @@
     </row>
     <row r="123" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A123" s="27" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="B123" t="s">
         <v>447</v>
@@ -17809,21 +17803,21 @@
     </row>
     <row r="124" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A124" s="27" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="B124" t="s">
+        <v>261</v>
+      </c>
+      <c r="C124" t="s">
         <v>449</v>
-      </c>
-      <c r="C124" t="s">
-        <v>450</v>
       </c>
     </row>
     <row r="125" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A125" s="27" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="B125" t="s">
-        <v>263</v>
+        <v>450</v>
       </c>
       <c r="C125" t="s">
         <v>451</v>
@@ -17831,7 +17825,7 @@
     </row>
     <row r="126" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A126" s="27" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="B126" t="s">
         <v>452</v>
@@ -17842,7 +17836,7 @@
     </row>
     <row r="127" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A127" s="27" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="B127" t="s">
         <v>454</v>
@@ -17853,7 +17847,7 @@
     </row>
     <row r="128" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A128" s="27" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="B128" t="s">
         <v>456</v>
@@ -17864,7 +17858,7 @@
     </row>
     <row r="129" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A129" s="27" t="s">
-        <v>83</v>
+        <v>158</v>
       </c>
       <c r="B129" t="s">
         <v>458</v>
@@ -17875,7 +17869,7 @@
     </row>
     <row r="130" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A130" s="27" t="s">
-        <v>158</v>
+        <v>84</v>
       </c>
       <c r="B130" t="s">
         <v>460</v>
@@ -17886,7 +17880,7 @@
     </row>
     <row r="131" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A131" s="27" t="s">
-        <v>84</v>
+        <v>159</v>
       </c>
       <c r="B131" t="s">
         <v>462</v>
@@ -17897,7 +17891,7 @@
     </row>
     <row r="132" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A132" s="27" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="B132" t="s">
         <v>464</v>
@@ -17908,7 +17902,7 @@
     </row>
     <row r="133" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A133" s="27" t="s">
-        <v>160</v>
+        <v>85</v>
       </c>
       <c r="B133" t="s">
         <v>466</v>
@@ -17919,7 +17913,7 @@
     </row>
     <row r="134" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A134" s="27" t="s">
-        <v>85</v>
+        <v>161</v>
       </c>
       <c r="B134" t="s">
         <v>468</v>
@@ -17930,7 +17924,7 @@
     </row>
     <row r="135" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A135" s="27" t="s">
-        <v>161</v>
+        <v>86</v>
       </c>
       <c r="B135" t="s">
         <v>470</v>
@@ -17941,7 +17935,7 @@
     </row>
     <row r="136" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A136" s="27" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="B136" t="s">
         <v>472</v>
@@ -17952,7 +17946,7 @@
     </row>
     <row r="137" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A137" s="27" t="s">
-        <v>87</v>
+        <v>162</v>
       </c>
       <c r="B137" t="s">
         <v>474</v>
@@ -17963,7 +17957,7 @@
     </row>
     <row r="138" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A138" s="27" t="s">
-        <v>162</v>
+        <v>88</v>
       </c>
       <c r="B138" t="s">
         <v>476</v>
@@ -17974,7 +17968,7 @@
     </row>
     <row r="139" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A139" s="27" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="B139" t="s">
         <v>478</v>
@@ -17985,7 +17979,7 @@
     </row>
     <row r="140" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A140" s="27" t="s">
-        <v>89</v>
+        <v>163</v>
       </c>
       <c r="B140" t="s">
         <v>480</v>
@@ -17996,7 +17990,7 @@
     </row>
     <row r="141" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A141" s="27" t="s">
-        <v>163</v>
+        <v>90</v>
       </c>
       <c r="B141" t="s">
         <v>482</v>
@@ -18007,29 +18001,29 @@
     </row>
     <row r="142" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A142" s="27" t="s">
-        <v>90</v>
+        <v>201</v>
       </c>
       <c r="B142" t="s">
-        <v>484</v>
+        <v>384</v>
       </c>
       <c r="C142" t="s">
-        <v>485</v>
+        <v>385</v>
       </c>
     </row>
     <row r="143" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A143" s="27" t="s">
-        <v>203</v>
+        <v>164</v>
       </c>
       <c r="B143" t="s">
-        <v>386</v>
+        <v>484</v>
       </c>
       <c r="C143" t="s">
-        <v>387</v>
+        <v>485</v>
       </c>
     </row>
     <row r="144" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A144" s="27" t="s">
-        <v>164</v>
+        <v>194</v>
       </c>
       <c r="B144" t="s">
         <v>486</v>
@@ -18040,7 +18034,7 @@
     </row>
     <row r="145" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A145" s="27" t="s">
-        <v>196</v>
+        <v>91</v>
       </c>
       <c r="B145" t="s">
         <v>488</v>
@@ -18051,7 +18045,7 @@
     </row>
     <row r="146" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A146" s="27" t="s">
-        <v>91</v>
+        <v>165</v>
       </c>
       <c r="B146" t="s">
         <v>490</v>
@@ -18062,7 +18056,7 @@
     </row>
     <row r="147" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A147" s="27" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="B147" t="s">
         <v>492</v>
@@ -18073,7 +18067,7 @@
     </row>
     <row r="148" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A148" s="27" t="s">
-        <v>166</v>
+        <v>92</v>
       </c>
       <c r="B148" t="s">
         <v>494</v>
@@ -18084,7 +18078,7 @@
     </row>
     <row r="149" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A149" s="27" t="s">
-        <v>92</v>
+        <v>167</v>
       </c>
       <c r="B149" t="s">
         <v>496</v>
@@ -18095,7 +18089,7 @@
     </row>
     <row r="150" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A150" s="27" t="s">
-        <v>167</v>
+        <v>25</v>
       </c>
       <c r="B150" t="s">
         <v>498</v>
@@ -18106,7 +18100,7 @@
     </row>
     <row r="151" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A151" s="27" t="s">
-        <v>25</v>
+        <v>168</v>
       </c>
       <c r="B151" t="s">
         <v>500</v>
@@ -18117,7 +18111,7 @@
     </row>
     <row r="152" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A152" s="27" t="s">
-        <v>168</v>
+        <v>206</v>
       </c>
       <c r="B152" t="s">
         <v>502</v>
@@ -18128,7 +18122,7 @@
     </row>
     <row r="153" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A153" s="27" t="s">
-        <v>208</v>
+        <v>170</v>
       </c>
       <c r="B153" t="s">
         <v>504</v>
@@ -18139,7 +18133,7 @@
     </row>
     <row r="154" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A154" s="27" t="s">
-        <v>170</v>
+        <v>190</v>
       </c>
       <c r="B154" t="s">
         <v>506</v>
@@ -18150,7 +18144,7 @@
     </row>
     <row r="155" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A155" s="27" t="s">
-        <v>192</v>
+        <v>93</v>
       </c>
       <c r="B155" t="s">
         <v>508</v>
@@ -18161,7 +18155,7 @@
     </row>
     <row r="156" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A156" s="27" t="s">
-        <v>93</v>
+        <v>193</v>
       </c>
       <c r="B156" t="s">
         <v>510</v>
@@ -18172,7 +18166,7 @@
     </row>
     <row r="157" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A157" s="27" t="s">
-        <v>195</v>
+        <v>171</v>
       </c>
       <c r="B157" t="s">
         <v>512</v>
@@ -18181,20 +18175,9 @@
         <v>513</v>
       </c>
     </row>
-    <row r="158" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A158" s="27" t="s">
-        <v>171</v>
-      </c>
-      <c r="B158" t="s">
-        <v>514</v>
-      </c>
-      <c r="C158" t="s">
-        <v>515</v>
-      </c>
-    </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C159">
-    <sortCondition ref="A2:A159"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C158">
+    <sortCondition ref="A2:A158"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>